<commit_message>
add column {MaHoaDonGoc}, TenNhanVien --> NguoiTao
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_PhieuTraHangNhap.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_PhieuTraHangNhap.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Trạng thái</t>
   </si>
@@ -28,9 +28,6 @@
     <t>DANH SÁCH TỔNG HỢP PHIẾU TRẢ HÀNG NHẬP</t>
   </si>
   <si>
-    <t>Mã trả hàng nhập</t>
-  </si>
-  <si>
     <t>Tên nhà cung cấp</t>
   </si>
   <si>
@@ -64,10 +61,16 @@
     <t>Tổng giảm giá</t>
   </si>
   <si>
-    <t>NV lập hóa đơn</t>
-  </si>
-  <si>
     <t>Tổng tiền thuế</t>
+  </si>
+  <si>
+    <t>Mã phiếu nhập</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn trả</t>
+  </si>
+  <si>
+    <t>User lập phiếu</t>
   </si>
 </sst>
 </file>
@@ -292,11 +295,11 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -603,534 +606,564 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="18" style="6" customWidth="1"/>
-    <col min="8" max="8" width="18" style="31" customWidth="1"/>
-    <col min="9" max="11" width="18" style="39" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="39" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" style="39" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" style="39" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" style="11" customWidth="1"/>
-    <col min="16" max="16" width="19" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="18" style="6" customWidth="1"/>
+    <col min="9" max="9" width="18" style="31" customWidth="1"/>
+    <col min="10" max="12" width="18" style="39" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" style="39" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="39" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" style="11" customWidth="1"/>
+    <col min="17" max="17" width="19" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="4" spans="1:16" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="4" spans="1:17" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="H4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K4" s="33" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" s="33" t="s">
+      <c r="O4" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="15"/>
-      <c r="D5" s="10"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="35"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="35"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="34"/>
       <c r="M5" s="35"/>
       <c r="N5" s="35"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="17"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O5" s="35"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="17"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="15"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="15"/>
-      <c r="D6" s="10"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="35"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="35"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="34"/>
       <c r="M6" s="35"/>
       <c r="N6" s="35"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="17"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O6" s="35"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="17"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="15"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="15"/>
-      <c r="D7" s="10"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="35"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="35"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="34"/>
       <c r="M7" s="35"/>
       <c r="N7" s="35"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="17"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O7" s="35"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="17"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="15"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="15"/>
-      <c r="D8" s="10"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="35"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="35"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="34"/>
       <c r="M8" s="35"/>
       <c r="N8" s="35"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="17"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O8" s="35"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="17"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="15"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="10"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="35"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="35"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="34"/>
       <c r="M9" s="35"/>
       <c r="N9" s="35"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="17"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O9" s="35"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="15"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="10"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="35"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="35"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="34"/>
       <c r="M10" s="35"/>
       <c r="N10" s="35"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="17"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O10" s="35"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="15"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="15"/>
-      <c r="D11" s="10"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="35"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="12"/>
       <c r="J11" s="35"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="34"/>
       <c r="M11" s="35"/>
       <c r="N11" s="35"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="17"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O11" s="35"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="17"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="15"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="10"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="35"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="35"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="34"/>
       <c r="M12" s="35"/>
       <c r="N12" s="35"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="17"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O12" s="35"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="17"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="15"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="10"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="35"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="35"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="34"/>
       <c r="M13" s="35"/>
       <c r="N13" s="35"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="17"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O13" s="35"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="17"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="15"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="35"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="35"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="34"/>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="17"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O14" s="35"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="17"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="15"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="15"/>
-      <c r="D15" s="10"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="35"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="35"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="34"/>
       <c r="M15" s="35"/>
       <c r="N15" s="35"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="17"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O15" s="35"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="17"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="15"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="15"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="35"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="35"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="34"/>
       <c r="M16" s="35"/>
       <c r="N16" s="35"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="17"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O16" s="35"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="17"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="15"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="15"/>
-      <c r="D17" s="10"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="35"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="35"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="34"/>
       <c r="M17" s="35"/>
       <c r="N17" s="35"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="17"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O17" s="35"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="17"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="15"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="15"/>
-      <c r="D18" s="10"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="35"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="12"/>
       <c r="J18" s="35"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="34"/>
       <c r="M18" s="35"/>
       <c r="N18" s="35"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="17"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O18" s="35"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="17"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="15"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="10"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="35"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="35"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="34"/>
       <c r="M19" s="35"/>
       <c r="N19" s="35"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="17"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O19" s="35"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="17"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="15"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="10"/>
+      <c r="D20" s="15"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="35"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="35"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="34"/>
       <c r="M20" s="35"/>
       <c r="N20" s="35"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="17"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O20" s="35"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="17"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="15"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="10"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="35"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="35"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="34"/>
       <c r="M21" s="35"/>
       <c r="N21" s="35"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="17"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O21" s="35"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="17"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="15"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="10"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="35"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="35"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="34"/>
       <c r="M22" s="35"/>
       <c r="N22" s="35"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="17"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O22" s="35"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="17"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="15"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="10"/>
+      <c r="D23" s="15"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="35"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="12"/>
       <c r="J23" s="35"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="34"/>
       <c r="M23" s="35"/>
       <c r="N23" s="35"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="17"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O23" s="35"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="17"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="15"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="10"/>
+      <c r="D24" s="15"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="35"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="12"/>
       <c r="J24" s="35"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="34"/>
       <c r="M24" s="35"/>
       <c r="N24" s="35"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="17"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O24" s="35"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="17"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="15"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="10"/>
+      <c r="D25" s="15"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="35"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="12"/>
       <c r="J25" s="35"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="34"/>
       <c r="M25" s="35"/>
       <c r="N25" s="35"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="17"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O25" s="35"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="17"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="15"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="15"/>
-      <c r="D26" s="10"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="35"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="12"/>
       <c r="J26" s="35"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="34"/>
       <c r="M26" s="35"/>
       <c r="N26" s="35"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="17"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O26" s="35"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="17"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="15"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="10"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="35"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="12"/>
       <c r="J27" s="35"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="34"/>
       <c r="M27" s="35"/>
       <c r="N27" s="35"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="17"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O27" s="35"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="17"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
+      <c r="B28" s="22"/>
       <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="37"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="26"/>
       <c r="J28" s="37"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="36"/>
       <c r="M28" s="37"/>
       <c r="N28" s="37"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="27"/>
-    </row>
-    <row r="29" spans="1:16" s="29" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O28" s="37"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="27"/>
+    </row>
+    <row r="29" spans="1:17" s="29" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -1138,16 +1171,13 @@
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="41">
-        <f xml:space="preserve"> SUM(I$5:I28)</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="41">
+      <c r="H29" s="21"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="40">
         <f xml:space="preserve"> SUM(J$5:J28)</f>
         <v>0</v>
       </c>
-      <c r="K29" s="38">
+      <c r="K29" s="40">
         <f xml:space="preserve"> SUM(K$5:K28)</f>
         <v>0</v>
       </c>
@@ -1163,12 +1193,16 @@
         <f xml:space="preserve"> SUM(N$5:N28)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="28"/>
-      <c r="P29" s="20"/>
+      <c r="O29" s="38">
+        <f xml:space="preserve"> SUM(O$5:O28)</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>